<commit_message>
utf-8-sig encoding to preprocessing
</commit_message>
<xml_diff>
--- a/preprocessing/sample_data.xlsx
+++ b/preprocessing/sample_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandraprinz/Desktop/junction2021/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandraprinz/Desktop/junction2021/preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD66BDB-47D3-5248-B028-A926B43DA0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948E874F-ECC6-D346-BCE6-12BA28D67548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="860" windowWidth="27820" windowHeight="19760" xr2:uid="{E43F782F-271A-2B4A-BFF4-571CF79397C7}"/>
+    <workbookView xWindow="9740" yWindow="1660" windowWidth="22300" windowHeight="18960" xr2:uid="{E43F782F-271A-2B4A-BFF4-571CF79397C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -890,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DEB094-E442-9940-9B3D-B8F8B15049F6}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>